<commit_message>
Added winvalues with recursive testing of moves.
</commit_message>
<xml_diff>
--- a/1.3_GameAI/Results.xlsx
+++ b/1.3_GameAI/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piet\Documents\GitHub\Game AI\1.3_GameAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DBA1BB-EAF1-422C-811A-537FB815B699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F708DFB1-C88E-4DFF-91C1-B496DF9A7476}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED9B9A0B-661D-4A86-8CA0-4C47376330DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Wins 1</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>Matchup, best of 100</t>
+  </si>
+  <si>
+    <t>Random++ vs Random+</t>
+  </si>
+  <si>
+    <t>Random++ vs Random++</t>
+  </si>
+  <si>
+    <t>Alpha 10 samplesize vs Random++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha 50 vs Random++ </t>
+  </si>
+  <si>
+    <t>Alpha 10 vs Alpha 50</t>
   </si>
 </sst>
 </file>
@@ -409,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE3BA00-31E8-4EA6-92CC-01A36B1633EF}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -464,6 +479,61 @@
         <v>41</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>